<commit_message>
Updated Sprint Planning Again
</commit_message>
<xml_diff>
--- a/Scrum/Scrum Sprint Planning.xlsx
+++ b/Scrum/Scrum Sprint Planning.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Sprint</t>
   </si>
   <si>
-    <t>Documentatie</t>
-  </si>
-  <si>
     <t>Register System, Login System, Account System, Websocket Chat, Friend System</t>
   </si>
   <si>
@@ -48,6 +45,12 @@
   </si>
   <si>
     <t>Contact information exchange, Business Job Offers, Business Accounts</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -116,17 +119,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -460,7 +453,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +466,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -484,10 +477,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,10 +488,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,10 +499,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,18 +510,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="y">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="y">
       <formula>NOT(ISERROR(SEARCH("y",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="n">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="n">
       <formula>NOT(ISERROR(SEARCH("n",C2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>